<commit_message>
add new command to vim cheatsheet
</commit_message>
<xml_diff>
--- a/vim cheatsheet by marvin.xlsx
+++ b/vim cheatsheet by marvin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\linux ubuntu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B62057-662C-43CF-B365-25A30B9C219E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4292EFA-74B4-49F1-A854-C023DAFDFE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>vi myfile</t>
   </si>
@@ -189,16 +189,7 @@
     <t>Delete the word at the current position</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Delete the rest of the current line</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>Delete the current line</t>
   </si>
   <si>
     <t>Delete N lines</t>
@@ -681,6 +672,33 @@
   </si>
   <si>
     <t>Nyy,yNy,yN</t>
+  </si>
+  <si>
+    <t>Substutute new for old</t>
+  </si>
+  <si>
+    <t>:s/old/new/g</t>
+  </si>
+  <si>
+    <t>Display cursor location</t>
+  </si>
+  <si>
+    <t>CTRL-g</t>
+  </si>
+  <si>
+    <t>dd, 2dd</t>
+  </si>
+  <si>
+    <t>Delete the current line; delete 2 lines</t>
+  </si>
+  <si>
+    <t>D or d$</t>
+  </si>
+  <si>
+    <t>2w</t>
+  </si>
+  <si>
+    <t>To move 2 words forward</t>
   </si>
 </sst>
 </file>
@@ -749,7 +767,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -813,11 +831,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -852,38 +894,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color rgb="FFFFFFFF"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1044,6 +1068,33 @@
         <top style="medium">
           <color rgb="FFFFFFFF"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color rgb="FFFFFFFF"/>
+        </vertical>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1060,12 +1111,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9BF7639-0F36-443B-8F93-A5425753D48E}" name="Table2" displayName="Table2" ref="A2:D25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9BF7639-0F36-443B-8F93-A5425753D48E}" name="Table2" displayName="Table2" ref="A2:D27" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{06C4FD9C-4020-4C25-9C64-9E92EADA66ED}" name="vi myfile" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{08EDD78D-8D66-46B3-ABE1-695AE17E9DE2}" name="Start the editor and edit myfile" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{AB9B230D-E5E0-4DC6-AC78-605D4EF2C3DE}" name="a" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{FBB37C0E-E0F5-4967-A008-CF6BB10F4DED}" name="Append text after cursor; stop upon Escape key" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{06C4FD9C-4020-4C25-9C64-9E92EADA66ED}" name="vi myfile" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{08EDD78D-8D66-46B3-ABE1-695AE17E9DE2}" name="Start the editor and edit myfile" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{AB9B230D-E5E0-4DC6-AC78-605D4EF2C3DE}" name="a" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FBB37C0E-E0F5-4967-A008-CF6BB10F4DED}" name="Append text after cursor; stop upon Escape key" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1334,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1355,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.8" thickBot="1">
@@ -1369,13 +1420,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" thickBot="1">
@@ -1383,13 +1434,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.8" thickBot="1">
@@ -1403,7 +1454,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.8" thickBot="1">
@@ -1411,13 +1462,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="31.8" thickBot="1">
@@ -1425,13 +1476,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.8" thickBot="1">
@@ -1459,7 +1510,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.8" thickBot="1">
@@ -1478,10 +1529,10 @@
     </row>
     <row r="11" spans="1:4" ht="31.8" thickBot="1">
       <c r="A11" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>49</v>
@@ -1502,16 +1553,16 @@
     </row>
     <row r="13" spans="1:4" ht="16.8" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.8" thickBot="1">
@@ -1522,38 +1573,38 @@
         <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.8" thickBot="1">
       <c r="A15" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.8" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.8" thickBot="1">
@@ -1564,10 +1615,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.8" thickBot="1">
@@ -1578,10 +1629,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30.6" thickBot="1">
@@ -1592,85 +1643,111 @@
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.8" thickBot="1">
       <c r="A20" s="7" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="16.8" thickBot="1">
       <c r="A21" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="16.8" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.8" thickBot="1">
+      <c r="A23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" thickBot="1">
-      <c r="A23" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="1:4" ht="17.399999999999999" thickBot="1">
+      <c r="A24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16.8" thickBot="1">
-      <c r="A24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.8" thickBot="1">
       <c r="A25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.8" thickBot="1">
+      <c r="A26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16.2">
+      <c r="A27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>